<commit_message>
little correction in sundar basti valuation for valuation in last tag
</commit_message>
<xml_diff>
--- a/ofc/estimates/finalized estimates/सुन्दर बस्ती सडक/valuation sundar basti.xlsx
+++ b/ofc/estimates/finalized estimates/सुन्दर बस्ती सडक/valuation sundar basti.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\finalized estimates\सुन्दर बस्ती सडक\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\finalized estimates\सुन्दर बस्ती सडक\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="estimate" sheetId="17" r:id="rId1"/>
     <sheet name="WCR" sheetId="6" r:id="rId2"/>
     <sheet name="valuated" sheetId="20" r:id="rId3"/>
-    <sheet name="M" sheetId="21" r:id="rId4"/>
+    <sheet name="M" sheetId="22" r:id="rId4"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
@@ -48,7 +48,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">valuated!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="66">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -182,9 +182,6 @@
     <t xml:space="preserve">Work Finished:           </t>
   </si>
   <si>
-    <t xml:space="preserve">Date:2079/06/13       </t>
-  </si>
-  <si>
     <t>VAT calculation</t>
   </si>
   <si>
@@ -261,15 +258,21 @@
   </si>
   <si>
     <t xml:space="preserve">F.Y:2081/2082           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date:2081/07/25       </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -438,7 +441,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -448,7 +451,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -468,14 +471,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -484,7 +487,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -509,7 +512,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -545,7 +548,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -554,7 +557,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -569,7 +572,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -591,7 +594,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -603,6 +606,24 @@
     </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -614,22 +635,19 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -651,21 +669,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1227,134 +1230,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S109"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:XFD52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="78" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="79" t="s">
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="79" t="s">
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-    </row>
-    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="80" t="s">
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="75" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="76" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="76"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="72" t="s">
+      <c r="H6" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="73" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="79" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1389,12 +1392,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>1</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
@@ -1406,10 +1409,10 @@
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="38">
         <v>1</v>
@@ -1440,10 +1443,10 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="38">
         <v>2</v>
@@ -1474,10 +1477,10 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
@@ -1488,7 +1491,7 @@
         <v>60.18829594999049</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I12" s="23">
         <v>64.63</v>
@@ -1506,10 +1509,10 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
@@ -1531,7 +1534,7 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="24"/>
       <c r="C14" s="19"/>
@@ -1551,12 +1554,12 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>2</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="20"/>
@@ -1575,7 +1578,7 @@
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
     </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="39" t="str">
         <f>B11</f>
@@ -1610,10 +1613,10 @@
       <c r="R16" s="25"/>
       <c r="S16" s="25"/>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="42"/>
       <c r="B17" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="44"/>
       <c r="D17" s="45"/>
@@ -1624,7 +1627,7 @@
         <v>0.53014376029327759</v>
       </c>
       <c r="H17" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I17" s="33">
         <v>4561.53</v>
@@ -1635,10 +1638,10 @@
       </c>
       <c r="K17" s="38"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="42"/>
       <c r="B18" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="44"/>
       <c r="D18" s="45"/>
@@ -1653,7 +1656,7 @@
       </c>
       <c r="K18" s="38"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="42"/>
       <c r="B19" s="39"/>
       <c r="C19" s="44"/>
@@ -1666,12 +1669,12 @@
       <c r="J19" s="47"/>
       <c r="K19" s="38"/>
     </row>
-    <row r="20" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>3</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="20"/>
@@ -1690,7 +1693,7 @@
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="39" t="str">
         <f>B16</f>
@@ -1724,10 +1727,10 @@
       <c r="R21" s="25"/>
       <c r="S21" s="25"/>
     </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="42"/>
       <c r="B22" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="44"/>
       <c r="D22" s="45"/>
@@ -1738,7 +1741,7 @@
         <v>0.26507188014663879</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I22" s="33">
         <v>10634.5</v>
@@ -1749,10 +1752,10 @@
       </c>
       <c r="K22" s="38"/>
     </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="42"/>
       <c r="B23" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="44"/>
       <c r="D23" s="45"/>
@@ -1767,7 +1770,7 @@
       </c>
       <c r="K23" s="38"/>
     </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="42"/>
       <c r="B24" s="39"/>
       <c r="C24" s="44"/>
@@ -1780,12 +1783,12 @@
       <c r="J24" s="47"/>
       <c r="K24" s="38"/>
     </row>
-    <row r="25" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>4</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="20"/>
@@ -1804,10 +1807,10 @@
       <c r="R25" s="25"/>
       <c r="S25" s="25"/>
     </row>
-    <row r="26" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="60">
         <v>2</v>
@@ -1831,10 +1834,10 @@
       <c r="R26" s="25"/>
       <c r="S26" s="25"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="42"/>
       <c r="B27" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" s="44"/>
       <c r="D27" s="45"/>
@@ -1845,7 +1848,7 @@
         <v>2</v>
       </c>
       <c r="H27" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I27" s="33">
         <v>7063</v>
@@ -1856,10 +1859,10 @@
       </c>
       <c r="K27" s="38"/>
     </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="42"/>
       <c r="B28" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="44"/>
       <c r="D28" s="45"/>
@@ -1874,7 +1877,7 @@
       </c>
       <c r="K28" s="38"/>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="42"/>
       <c r="B29" s="39"/>
       <c r="C29" s="44"/>
@@ -1887,12 +1890,12 @@
       <c r="J29" s="47"/>
       <c r="K29" s="38"/>
     </row>
-    <row r="30" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A30" s="18">
         <v>5</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="20"/>
@@ -1911,7 +1914,7 @@
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="39" t="str">
         <f>B26</f>
@@ -1946,10 +1949,10 @@
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" s="60">
         <f>-2*2-1</f>
@@ -1986,10 +1989,10 @@
       <c r="R32" s="25"/>
       <c r="S32" s="25"/>
     </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="42"/>
       <c r="B33" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33" s="44"/>
       <c r="D33" s="45"/>
@@ -2000,7 +2003,7 @@
         <v>1.4627309973224794</v>
       </c>
       <c r="H33" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I33" s="33">
         <v>14362.76</v>
@@ -2023,10 +2026,10 @@
         <v>0.58473026516306004</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="42"/>
       <c r="B34" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34" s="44"/>
       <c r="D34" s="45"/>
@@ -2041,7 +2044,7 @@
       </c>
       <c r="K34" s="38"/>
     </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="42"/>
       <c r="B35" s="39"/>
       <c r="C35" s="44"/>
@@ -2054,12 +2057,12 @@
       <c r="J35" s="47"/>
       <c r="K35" s="38"/>
     </row>
-    <row r="36" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="18">
         <v>6</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" s="38"/>
       <c r="D36" s="40"/>
@@ -2078,10 +2081,10 @@
       <c r="R36" s="25"/>
       <c r="S36" s="25"/>
     </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37" s="38">
         <f>(45+17.5)/2.5+1</f>
@@ -2117,10 +2120,10 @@
       <c r="R37" s="25"/>
       <c r="S37" s="25"/>
     </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>
       <c r="B38" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" s="38"/>
       <c r="D38" s="40"/>
@@ -2131,7 +2134,7 @@
         <v>65</v>
       </c>
       <c r="H38" s="42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I38" s="42">
         <v>6932.79</v>
@@ -2152,10 +2155,10 @@
       <c r="R38" s="25"/>
       <c r="S38" s="25"/>
     </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C39" s="38"/>
       <c r="D39" s="40"/>
@@ -2177,7 +2180,7 @@
       <c r="R39" s="25"/>
       <c r="S39" s="25"/>
     </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="39"/>
       <c r="C40" s="38"/>
@@ -2197,12 +2200,12 @@
       <c r="R40" s="25"/>
       <c r="S40" s="25"/>
     </row>
-    <row r="41" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="18">
         <v>7</v>
       </c>
       <c r="B41" s="67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41" s="38">
         <v>1</v>
@@ -2215,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="H41" s="42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I41" s="23">
         <v>5000</v>
@@ -2233,7 +2236,7 @@
       <c r="R41" s="25"/>
       <c r="S41" s="25"/>
     </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="39"/>
       <c r="C42" s="38"/>
@@ -2253,7 +2256,7 @@
       <c r="R42" s="25"/>
       <c r="S42" s="25"/>
     </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18">
         <v>8</v>
       </c>
@@ -2289,7 +2292,7 @@
       <c r="R43" s="25"/>
       <c r="S43" s="25"/>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="24"/>
       <c r="C44" s="19"/>
@@ -2309,7 +2312,7 @@
       <c r="R44" s="25"/>
       <c r="S44" s="25"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="42"/>
       <c r="B45" s="48" t="s">
         <v>17</v>
@@ -2327,7 +2330,7 @@
       </c>
       <c r="K45" s="38"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="62"/>
       <c r="B46" s="65"/>
       <c r="C46" s="66"/>
@@ -2340,16 +2343,16 @@
       <c r="J46" s="64"/>
       <c r="K46" s="59"/>
     </row>
-    <row r="47" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="52"/>
       <c r="B47" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C47" s="71">
+      <c r="C47" s="77">
         <f>J45</f>
         <v>558845.82475410122</v>
       </c>
-      <c r="D47" s="71"/>
+      <c r="D47" s="77"/>
       <c r="E47" s="41">
         <v>100</v>
       </c>
@@ -2360,15 +2363,15 @@
       <c r="J47" s="56"/>
       <c r="K47" s="57"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="58"/>
       <c r="B48" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C48" s="74">
+      <c r="C48" s="80">
         <v>500000</v>
       </c>
-      <c r="D48" s="74"/>
+      <c r="D48" s="80"/>
       <c r="E48" s="41"/>
       <c r="F48" s="51"/>
       <c r="G48" s="50"/>
@@ -2377,16 +2380,16 @@
       <c r="J48" s="50"/>
       <c r="K48" s="51"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="58"/>
       <c r="B49" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="74">
+      <c r="C49" s="80">
         <f>C48-C51-C52</f>
         <v>475000</v>
       </c>
-      <c r="D49" s="74"/>
+      <c r="D49" s="80"/>
       <c r="E49" s="41">
         <f>C49/C47*100</f>
         <v>84.996608896381332</v>
@@ -2398,16 +2401,16 @@
       <c r="J49" s="50"/>
       <c r="K49" s="51"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="58"/>
       <c r="B50" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="71">
+      <c r="C50" s="77">
         <f>C47-C49</f>
         <v>83845.824754101224</v>
       </c>
-      <c r="D50" s="71"/>
+      <c r="D50" s="77"/>
       <c r="E50" s="41">
         <f>100-E49</f>
         <v>15.003391103618668</v>
@@ -2419,16 +2422,16 @@
       <c r="J50" s="50"/>
       <c r="K50" s="51"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="58"/>
       <c r="B51" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C51" s="71">
+      <c r="C51" s="77">
         <f>C48*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D51" s="71"/>
+      <c r="D51" s="77"/>
       <c r="E51" s="41">
         <v>3</v>
       </c>
@@ -2439,16 +2442,16 @@
       <c r="J51" s="50"/>
       <c r="K51" s="51"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="58"/>
       <c r="B52" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C52" s="71">
+      <c r="C52" s="77">
         <f>C48*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D52" s="71"/>
+      <c r="D52" s="77"/>
       <c r="E52" s="41">
         <v>2</v>
       </c>
@@ -2459,7 +2462,7 @@
       <c r="J52" s="50"/>
       <c r="K52" s="51"/>
     </row>
-    <row r="53" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="59"/>
       <c r="B53" s="59"/>
       <c r="C53" s="59"/>
@@ -2472,71 +2475,64 @@
       <c r="J53" s="59"/>
       <c r="K53" s="59"/>
     </row>
-    <row r="54" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="102" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="103" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="104" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="105" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="106" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="107" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="108" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="109" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="A7:F7"/>
@@ -2545,6 +2541,13 @@
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="C50:D50"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -2561,110 +2564,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="90" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-    </row>
-    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="91" t="s">
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+    </row>
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="79" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="79" t="s">
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="92" t="s">
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="88">
+      <c r="C6" s="81">
         <f>F35</f>
         <v>558845.82475410122</v>
       </c>
-      <c r="D6" s="89"/>
+      <c r="D6" s="82"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -2672,90 +2675,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="88">
+      <c r="J6" s="81">
         <f>I35</f>
-        <v>560165.0746088404</v>
-      </c>
-      <c r="K6" s="89"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>559435.28089170333</v>
+      </c>
+      <c r="K6" s="82"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="I7" s="84" t="s">
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="I7" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="75" t="str">
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="71" t="str">
         <f>estimate!A6</f>
         <v xml:space="preserve">Project:- सुन्दरबस्ती सडक ग्राबेल र ढलान (ढल निर्माण कार्य) </v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="I8" s="85" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="86" t="str">
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="I8" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="91" t="str">
         <f>estimate!A7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="I9" s="85" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="81" t="s">
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
+      <c r="I9" s="90" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="81" t="s">
+      <c r="C11" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="87" t="s">
+      <c r="D11" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="87"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="87" t="s">
+      <c r="E11" s="92"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="87"/>
-      <c r="I11" s="87"/>
-      <c r="J11" s="81" t="s">
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="82" t="s">
+      <c r="K11" s="87" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="81"/>
-      <c r="B12" s="81"/>
-      <c r="C12" s="81"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="86"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="86"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -2774,10 +2777,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="81"/>
-      <c r="K12" s="82"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="J12" s="86"/>
+      <c r="K12" s="87"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
         <f>estimate!A9</f>
         <v>1</v>
@@ -2820,7 +2823,7 @@
       </c>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="70" t="str">
         <f>estimate!B13</f>
@@ -2845,7 +2848,7 @@
       </c>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="27"/>
       <c r="B15" s="32"/>
       <c r="C15" s="12"/>
@@ -2858,7 +2861,7 @@
       <c r="J15" s="28"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
         <f>estimate!A15</f>
         <v>2</v>
@@ -2901,7 +2904,7 @@
       </c>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
       <c r="B17" s="70" t="str">
         <f>estimate!B18</f>
@@ -2926,7 +2929,7 @@
       </c>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="27"/>
       <c r="B18" s="32"/>
       <c r="C18" s="12"/>
@@ -2939,7 +2942,7 @@
       <c r="J18" s="28"/>
       <c r="K18" s="14"/>
     </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
         <f>estimate!A20</f>
         <v>3</v>
@@ -2982,7 +2985,7 @@
       </c>
       <c r="K19" s="14"/>
     </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="27"/>
       <c r="B20" s="70" t="str">
         <f>estimate!B23</f>
@@ -3007,7 +3010,7 @@
       </c>
       <c r="K20" s="14"/>
     </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
       <c r="B21" s="32"/>
       <c r="C21" s="12"/>
@@ -3020,7 +3023,7 @@
       <c r="J21" s="28"/>
       <c r="K21" s="14"/>
     </row>
-    <row r="22" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
         <f>estimate!A25</f>
         <v>4</v>
@@ -3063,7 +3066,7 @@
       </c>
       <c r="K22" s="14"/>
     </row>
-    <row r="23" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="27"/>
       <c r="B23" s="70" t="str">
         <f>estimate!B28</f>
@@ -3088,7 +3091,7 @@
       </c>
       <c r="K23" s="14"/>
     </row>
-    <row r="24" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="27"/>
       <c r="B24" s="32"/>
       <c r="C24" s="12"/>
@@ -3101,7 +3104,7 @@
       <c r="J24" s="28"/>
       <c r="K24" s="14"/>
     </row>
-    <row r="25" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="27">
         <f>estimate!A30</f>
         <v>5</v>
@@ -3128,7 +3131,7 @@
       </c>
       <c r="G25" s="12">
         <f>valuated!G38</f>
-        <v>1.5566106253545435</v>
+        <v>1.5101366766636579</v>
       </c>
       <c r="H25" s="12">
         <f>valuated!I38</f>
@@ -3136,15 +3139,15 @@
       </c>
       <c r="I25" s="12">
         <f>G25*H25</f>
-        <v>22357.224825417223</v>
+        <v>21689.73065411772</v>
       </c>
       <c r="J25" s="28">
         <f>I25-F25</f>
-        <v>1348.3705663138098</v>
+        <v>680.87639501430749</v>
       </c>
       <c r="K25" s="14"/>
     </row>
-    <row r="26" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="27"/>
       <c r="B26" s="70" t="str">
         <f>estimate!B34</f>
@@ -3161,15 +3164,15 @@
       <c r="H26" s="12"/>
       <c r="I26" s="12">
         <f>valuated!J39</f>
-        <v>2086.6773264861499</v>
+        <v>2024.3777806485621</v>
       </c>
       <c r="J26" s="28">
         <f>I26-F26</f>
-        <v>125.8481010232365</v>
+        <v>63.548555185648638</v>
       </c>
       <c r="K26" s="14"/>
     </row>
-    <row r="27" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="27"/>
       <c r="B27" s="32"/>
       <c r="C27" s="12"/>
@@ -3182,7 +3185,7 @@
       <c r="J27" s="28"/>
       <c r="K27" s="14"/>
     </row>
-    <row r="28" spans="1:11" s="1" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A28" s="27">
         <f>estimate!A36</f>
         <v>6</v>
@@ -3225,7 +3228,7 @@
       </c>
       <c r="K28" s="14"/>
     </row>
-    <row r="29" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
       <c r="B29" s="70" t="str">
         <f>estimate!B39</f>
@@ -3250,7 +3253,7 @@
       </c>
       <c r="K29" s="14"/>
     </row>
-    <row r="30" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="27"/>
       <c r="B30" s="32"/>
       <c r="C30" s="12"/>
@@ -3263,7 +3266,7 @@
       <c r="J30" s="28"/>
       <c r="K30" s="14"/>
     </row>
-    <row r="31" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
         <f>estimate!A41</f>
         <v>7</v>
@@ -3306,7 +3309,7 @@
       </c>
       <c r="K31" s="14"/>
     </row>
-    <row r="32" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="27"/>
       <c r="B32" s="32"/>
       <c r="C32" s="12"/>
@@ -3319,7 +3322,7 @@
       <c r="J32" s="28"/>
       <c r="K32" s="14"/>
     </row>
-    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27">
         <f>estimate!A43</f>
         <v>8</v>
@@ -3362,7 +3365,7 @@
       </c>
       <c r="K33" s="14"/>
     </row>
-    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29"/>
       <c r="B34" s="29"/>
       <c r="C34" s="12"/>
@@ -3375,7 +3378,7 @@
       <c r="J34" s="28"/>
       <c r="K34" s="14"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="6" t="s">
         <v>16</v>
@@ -3391,23 +3394,16 @@
       <c r="H35" s="7"/>
       <c r="I35" s="7">
         <f>SUM(I13:I33)</f>
-        <v>560165.0746088404</v>
+        <v>559435.28089170333</v>
       </c>
       <c r="J35" s="13">
         <f>I35-F35</f>
-        <v>1319.2498547391733</v>
+        <v>589.45613760210108</v>
       </c>
       <c r="K35" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -3421,6 +3417,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3438,134 +3441,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S114"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A31" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q46" sqref="Q46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="78" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="79" t="s">
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="79" t="s">
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-    </row>
-    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="80" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="75" t="s">
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="76" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="76"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="72" t="s">
+      <c r="H6" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="73" t="s">
-        <v>63</v>
-      </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -3600,12 +3603,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>1</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
@@ -3617,10 +3620,10 @@
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="38">
         <v>1</v>
@@ -3651,10 +3654,10 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="38">
         <v>1</v>
@@ -3685,7 +3688,7 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="39"/>
       <c r="C12" s="38">
@@ -3716,10 +3719,10 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
@@ -3730,7 +3733,7 @@
         <v>72.425608007933732</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I13" s="23">
         <v>64.63</v>
@@ -3748,10 +3751,10 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
@@ -3773,7 +3776,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="24"/>
       <c r="C15" s="19"/>
@@ -3793,12 +3796,12 @@
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
     </row>
-    <row r="16" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>2</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
@@ -3817,7 +3820,7 @@
       <c r="R16" s="25"/>
       <c r="S16" s="25"/>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="39" t="str">
         <f>B11</f>
@@ -3852,7 +3855,7 @@
       <c r="R17" s="25"/>
       <c r="S17" s="25"/>
     </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="39"/>
       <c r="C18" s="38">
@@ -3884,10 +3887,10 @@
       <c r="R18" s="25"/>
       <c r="S18" s="25"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42"/>
       <c r="B19" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="44"/>
       <c r="D19" s="45"/>
@@ -3898,7 +3901,7 @@
         <v>0.43471788344048762</v>
       </c>
       <c r="H19" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I19" s="33">
         <v>4561.53</v>
@@ -3909,10 +3912,10 @@
       </c>
       <c r="K19" s="38"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="42"/>
       <c r="B20" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="44"/>
       <c r="D20" s="45"/>
@@ -3927,7 +3930,7 @@
       </c>
       <c r="K20" s="38"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="42"/>
       <c r="B21" s="39"/>
       <c r="C21" s="44"/>
@@ -3940,12 +3943,12 @@
       <c r="J21" s="47"/>
       <c r="K21" s="38"/>
     </row>
-    <row r="22" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>3</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="20"/>
@@ -3964,7 +3967,7 @@
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
     </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="39" t="str">
         <f>B17</f>
@@ -3998,7 +4001,7 @@
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
     </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="39"/>
       <c r="C24" s="38">
@@ -4029,10 +4032,10 @@
       <c r="R24" s="25"/>
       <c r="S24" s="25"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="42"/>
       <c r="B25" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="44"/>
       <c r="D25" s="45"/>
@@ -4043,7 +4046,7 @@
         <v>0.21735894172024381</v>
       </c>
       <c r="H25" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I25" s="33">
         <v>10634.5</v>
@@ -4054,10 +4057,10 @@
       </c>
       <c r="K25" s="38"/>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="42"/>
       <c r="B26" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="44"/>
       <c r="D26" s="45"/>
@@ -4072,7 +4075,7 @@
       </c>
       <c r="K26" s="38"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="42"/>
       <c r="B27" s="39"/>
       <c r="C27" s="44"/>
@@ -4085,12 +4088,12 @@
       <c r="J27" s="47"/>
       <c r="K27" s="38"/>
     </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="42">
         <v>4</v>
       </c>
       <c r="B28" s="67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" s="44"/>
       <c r="D28" s="45"/>
@@ -4102,10 +4105,10 @@
       <c r="J28" s="46"/>
       <c r="K28" s="38"/>
     </row>
-    <row r="29" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="60">
         <v>2</v>
@@ -4129,10 +4132,10 @@
       <c r="R29" s="25"/>
       <c r="S29" s="25"/>
     </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="42"/>
       <c r="B30" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="44"/>
       <c r="D30" s="45"/>
@@ -4143,7 +4146,7 @@
         <v>2</v>
       </c>
       <c r="H30" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I30" s="33">
         <v>7063</v>
@@ -4154,10 +4157,10 @@
       </c>
       <c r="K30" s="38"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="42"/>
       <c r="B31" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="44"/>
       <c r="D31" s="45"/>
@@ -4172,7 +4175,7 @@
       </c>
       <c r="K31" s="38"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="42"/>
       <c r="B32" s="39"/>
       <c r="C32" s="44"/>
@@ -4185,12 +4188,12 @@
       <c r="J32" s="47"/>
       <c r="K32" s="38"/>
     </row>
-    <row r="33" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
         <v>5</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="20"/>
@@ -4209,7 +4212,7 @@
       <c r="R33" s="25"/>
       <c r="S33" s="25"/>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="39" t="str">
         <f>B23</f>
@@ -4219,19 +4222,19 @@
         <v>1</v>
       </c>
       <c r="D34" s="61">
-        <f>((1.5-0.23)+(((23+6)/12/3.281)-0.23))/2</f>
-        <v>0.88828202783704158</v>
+        <f>((1.5-0.23)+(((33)/12/3.281)-0.23))/2</f>
+        <v>0.93907954891801282</v>
       </c>
       <c r="E34" s="61">
         <v>0.23</v>
       </c>
       <c r="F34" s="61">
-        <f>6.33/3.281</f>
-        <v>1.929289850655288</v>
+        <f>6/3.281</f>
+        <v>1.8287107589149649</v>
       </c>
       <c r="G34" s="41">
         <f>C34*(PI())*(D34)*E34*F34</f>
-        <v>1.2383005438991532</v>
+        <v>1.2408666469319718</v>
       </c>
       <c r="H34" s="42"/>
       <c r="I34" s="42"/>
@@ -4245,10 +4248,10 @@
       <c r="R34" s="25"/>
       <c r="S34" s="25"/>
     </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" s="60">
         <v>-3</v>
@@ -4284,7 +4287,7 @@
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="39" t="str">
         <f>B34</f>
@@ -4301,12 +4304,12 @@
         <v>0.23</v>
       </c>
       <c r="F36" s="61">
-        <f>4.33/3.281</f>
-        <v>1.3197195976836329</v>
+        <f>4/3.281</f>
+        <v>1.2191405059433098</v>
       </c>
       <c r="G36" s="41">
         <f>C36*(PI())*(D36)*E36*F36</f>
-        <v>0.64346492110193376</v>
+        <v>0.5944248693782298</v>
       </c>
       <c r="H36" s="42"/>
       <c r="I36" s="42"/>
@@ -4320,10 +4323,10 @@
       <c r="R36" s="25"/>
       <c r="S36" s="25"/>
     </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="60">
         <v>-2</v>
@@ -4359,10 +4362,10 @@
       <c r="R37" s="25"/>
       <c r="S37" s="25"/>
     </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="42"/>
       <c r="B38" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" s="44"/>
       <c r="D38" s="45"/>
@@ -4370,17 +4373,17 @@
       <c r="F38" s="45"/>
       <c r="G38" s="33">
         <f>SUM(G34:G37)</f>
-        <v>1.5566106253545435</v>
+        <v>1.5101366766636579</v>
       </c>
       <c r="H38" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I38" s="33">
         <v>14362.76</v>
       </c>
       <c r="J38" s="46">
         <f>G38*I38</f>
-        <v>22357.224825417223</v>
+        <v>21689.73065411772</v>
       </c>
       <c r="K38" s="38"/>
       <c r="N38">
@@ -4396,10 +4399,10 @@
         <v>0.58473026516306004</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="42"/>
       <c r="B39" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C39" s="44"/>
       <c r="D39" s="45"/>
@@ -4410,11 +4413,11 @@
       <c r="I39" s="45"/>
       <c r="J39" s="47">
         <f>0.13*G38*10311.74</f>
-        <v>2086.6773264861499</v>
+        <v>2024.3777806485621</v>
       </c>
       <c r="K39" s="38"/>
     </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="42"/>
       <c r="B40" s="39"/>
       <c r="C40" s="44"/>
@@ -4427,12 +4430,12 @@
       <c r="J40" s="47"/>
       <c r="K40" s="38"/>
     </row>
-    <row r="41" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="18">
         <v>6</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="38"/>
       <c r="D41" s="40"/>
@@ -4451,10 +4454,10 @@
       <c r="R41" s="25"/>
       <c r="S41" s="25"/>
     </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C42" s="38">
         <f>(45+17.5)/2.5+1</f>
@@ -4490,10 +4493,10 @@
       <c r="R42" s="25"/>
       <c r="S42" s="25"/>
     </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18"/>
       <c r="B43" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43" s="38"/>
       <c r="D43" s="40"/>
@@ -4504,7 +4507,7 @@
         <v>65</v>
       </c>
       <c r="H43" s="42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I43" s="42">
         <v>6932.79</v>
@@ -4525,10 +4528,10 @@
       <c r="R43" s="25"/>
       <c r="S43" s="25"/>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C44" s="38"/>
       <c r="D44" s="40"/>
@@ -4550,7 +4553,7 @@
       <c r="R44" s="25"/>
       <c r="S44" s="25"/>
     </row>
-    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="39"/>
       <c r="C45" s="38"/>
@@ -4570,12 +4573,12 @@
       <c r="R45" s="25"/>
       <c r="S45" s="25"/>
     </row>
-    <row r="46" spans="1:19" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="18">
         <v>7</v>
       </c>
       <c r="B46" s="68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" s="29">
         <v>1</v>
@@ -4588,7 +4591,7 @@
         <v>1</v>
       </c>
       <c r="H46" s="69" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I46" s="23">
         <v>5000</v>
@@ -4602,7 +4605,7 @@
       <c r="R46" s="35"/>
       <c r="S46" s="35"/>
     </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
       <c r="B47" s="39"/>
       <c r="C47" s="38"/>
@@ -4622,7 +4625,7 @@
       <c r="R47" s="25"/>
       <c r="S47" s="25"/>
     </row>
-    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18">
         <v>8</v>
       </c>
@@ -4658,7 +4661,7 @@
       <c r="R48" s="25"/>
       <c r="S48" s="25"/>
     </row>
-    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18"/>
       <c r="B49" s="24"/>
       <c r="C49" s="19"/>
@@ -4678,7 +4681,7 @@
       <c r="R49" s="25"/>
       <c r="S49" s="25"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="42"/>
       <c r="B50" s="48" t="s">
         <v>17</v>
@@ -4692,11 +4695,11 @@
       <c r="I50" s="43"/>
       <c r="J50" s="43">
         <f>SUM(J10:J48)</f>
-        <v>560165.0746088404</v>
+        <v>559435.28089170333</v>
       </c>
       <c r="K50" s="38"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="62"/>
       <c r="B51" s="65"/>
       <c r="C51" s="66"/>
@@ -4709,16 +4712,16 @@
       <c r="J51" s="64"/>
       <c r="K51" s="59"/>
     </row>
-    <row r="52" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="52"/>
       <c r="B52" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" s="71">
+        <v>60</v>
+      </c>
+      <c r="C52" s="77">
         <f>J50</f>
-        <v>560165.0746088404</v>
-      </c>
-      <c r="D52" s="71"/>
+        <v>559435.28089170333</v>
+      </c>
+      <c r="D52" s="77"/>
       <c r="E52" s="41">
         <v>100</v>
       </c>
@@ -4729,15 +4732,15 @@
       <c r="J52" s="56"/>
       <c r="K52" s="57"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="58"/>
       <c r="B53" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C53" s="74">
+      <c r="C53" s="80">
         <v>500000</v>
       </c>
-      <c r="D53" s="74"/>
+      <c r="D53" s="80"/>
       <c r="E53" s="41"/>
       <c r="F53" s="51"/>
       <c r="G53" s="50"/>
@@ -4746,40 +4749,42 @@
       <c r="J53" s="50"/>
       <c r="K53" s="51"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="58"/>
       <c r="B54" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C54" s="74">
-        <f>0.85*C52</f>
-        <v>476140.31341751432</v>
-      </c>
-      <c r="D54" s="74"/>
+      <c r="C54" s="80">
+        <f>C53-C56-C57</f>
+        <v>475000</v>
+      </c>
+      <c r="D54" s="80"/>
       <c r="E54" s="41">
         <f>C54/C52*100</f>
-        <v>85</v>
+        <v>84.907051132506524</v>
       </c>
       <c r="F54" s="51"/>
       <c r="G54" s="50"/>
       <c r="H54" s="50"/>
-      <c r="I54" s="50"/>
+      <c r="I54" s="50" t="s">
+        <v>65</v>
+      </c>
       <c r="J54" s="50"/>
       <c r="K54" s="51"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="58"/>
       <c r="B55" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C55" s="71">
+      <c r="C55" s="77">
         <f>C52-C54</f>
-        <v>84024.761191326077</v>
-      </c>
-      <c r="D55" s="71"/>
+        <v>84435.280891703325</v>
+      </c>
+      <c r="D55" s="77"/>
       <c r="E55" s="41">
         <f>100-E54</f>
-        <v>15</v>
+        <v>15.092948867493476</v>
       </c>
       <c r="F55" s="51"/>
       <c r="G55" s="50"/>
@@ -4788,16 +4793,16 @@
       <c r="J55" s="50"/>
       <c r="K55" s="51"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="58"/>
       <c r="B56" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="71">
+      <c r="C56" s="77">
         <f>C53*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D56" s="71"/>
+      <c r="D56" s="77"/>
       <c r="E56" s="41">
         <v>3</v>
       </c>
@@ -4808,16 +4813,16 @@
       <c r="J56" s="50"/>
       <c r="K56" s="51"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="58"/>
       <c r="B57" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C57" s="71">
+      <c r="C57" s="77">
         <f>C53*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D57" s="71"/>
+      <c r="D57" s="77"/>
       <c r="E57" s="41">
         <v>2</v>
       </c>
@@ -4828,7 +4833,7 @@
       <c r="J57" s="50"/>
       <c r="K57" s="51"/>
     </row>
-    <row r="58" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="59"/>
       <c r="B58" s="59"/>
       <c r="C58" s="59"/>
@@ -4841,64 +4846,71 @@
       <c r="J58" s="59"/>
       <c r="K58" s="59"/>
     </row>
-    <row r="59" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="102" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="103" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="104" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="105" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="106" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="107" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="108" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="109" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="110" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="111" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="112" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="113" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="114" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="A7:F7"/>
@@ -4907,13 +4919,6 @@
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="C55:D55"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -4930,134 +4935,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S114"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A22" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="78" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="79" t="s">
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="79" t="s">
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-    </row>
-    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="80" t="s">
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="76" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="75" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="76" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="76"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="72" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="73" t="s">
-        <v>63</v>
-      </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="79"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -5092,12 +5097,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>1</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
@@ -5109,10 +5114,10 @@
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="38">
         <v>1</v>
@@ -5143,10 +5148,10 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="38">
         <v>1</v>
@@ -5177,7 +5182,7 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="39"/>
       <c r="C12" s="38">
@@ -5208,10 +5213,10 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
@@ -5222,7 +5227,7 @@
         <v>72.425608007933732</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I13" s="23">
         <v>64.63</v>
@@ -5240,10 +5245,10 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
@@ -5265,7 +5270,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="24"/>
       <c r="C15" s="19"/>
@@ -5285,12 +5290,12 @@
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
     </row>
-    <row r="16" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>2</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
@@ -5309,7 +5314,7 @@
       <c r="R16" s="25"/>
       <c r="S16" s="25"/>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="39" t="str">
         <f>B11</f>
@@ -5344,7 +5349,7 @@
       <c r="R17" s="25"/>
       <c r="S17" s="25"/>
     </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="39"/>
       <c r="C18" s="38">
@@ -5376,10 +5381,10 @@
       <c r="R18" s="25"/>
       <c r="S18" s="25"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42"/>
       <c r="B19" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="44"/>
       <c r="D19" s="45"/>
@@ -5390,7 +5395,7 @@
         <v>0.43471788344048762</v>
       </c>
       <c r="H19" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I19" s="33">
         <v>4561.53</v>
@@ -5401,10 +5406,10 @@
       </c>
       <c r="K19" s="38"/>
     </row>
-    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="42"/>
       <c r="B20" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="44"/>
       <c r="D20" s="45"/>
@@ -5419,7 +5424,7 @@
       </c>
       <c r="K20" s="38"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="42"/>
       <c r="B21" s="39"/>
       <c r="C21" s="44"/>
@@ -5432,12 +5437,12 @@
       <c r="J21" s="47"/>
       <c r="K21" s="38"/>
     </row>
-    <row r="22" spans="1:19" ht="69" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>3</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="20"/>
@@ -5456,7 +5461,7 @@
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
     </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="39" t="str">
         <f>B17</f>
@@ -5490,7 +5495,7 @@
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
     </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="39"/>
       <c r="C24" s="38">
@@ -5521,10 +5526,10 @@
       <c r="R24" s="25"/>
       <c r="S24" s="25"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="42"/>
       <c r="B25" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="44"/>
       <c r="D25" s="45"/>
@@ -5535,7 +5540,7 @@
         <v>0.21735894172024381</v>
       </c>
       <c r="H25" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I25" s="33">
         <v>10634.5</v>
@@ -5546,10 +5551,10 @@
       </c>
       <c r="K25" s="38"/>
     </row>
-    <row r="26" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="42"/>
       <c r="B26" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="44"/>
       <c r="D26" s="45"/>
@@ -5564,7 +5569,7 @@
       </c>
       <c r="K26" s="38"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="42"/>
       <c r="B27" s="39"/>
       <c r="C27" s="44"/>
@@ -5577,12 +5582,12 @@
       <c r="J27" s="47"/>
       <c r="K27" s="38"/>
     </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="42">
         <v>4</v>
       </c>
       <c r="B28" s="67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" s="44"/>
       <c r="D28" s="45"/>
@@ -5594,10 +5599,10 @@
       <c r="J28" s="46"/>
       <c r="K28" s="38"/>
     </row>
-    <row r="29" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="60">
         <v>2</v>
@@ -5621,10 +5626,10 @@
       <c r="R29" s="25"/>
       <c r="S29" s="25"/>
     </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="42"/>
       <c r="B30" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="44"/>
       <c r="D30" s="45"/>
@@ -5635,7 +5640,7 @@
         <v>2</v>
       </c>
       <c r="H30" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I30" s="33">
         <v>7063</v>
@@ -5646,10 +5651,10 @@
       </c>
       <c r="K30" s="38"/>
     </row>
-    <row r="31" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="42"/>
       <c r="B31" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="44"/>
       <c r="D31" s="45"/>
@@ -5664,7 +5669,7 @@
       </c>
       <c r="K31" s="38"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="42"/>
       <c r="B32" s="39"/>
       <c r="C32" s="44"/>
@@ -5677,12 +5682,12 @@
       <c r="J32" s="47"/>
       <c r="K32" s="38"/>
     </row>
-    <row r="33" spans="1:19" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
         <v>5</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="20"/>
@@ -5701,7 +5706,7 @@
       <c r="R33" s="25"/>
       <c r="S33" s="25"/>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="39" t="str">
         <f>B23</f>
@@ -5711,19 +5716,19 @@
         <v>1</v>
       </c>
       <c r="D34" s="61">
-        <f>((1.5-0.23)+(((23+6)/12/3.281)-0.23))/2</f>
-        <v>0.88828202783704158</v>
+        <f>((1.5-0.23)+(((33)/12/3.281)-0.23))/2</f>
+        <v>0.93907954891801282</v>
       </c>
       <c r="E34" s="61">
         <v>0.23</v>
       </c>
       <c r="F34" s="61">
-        <f>6.33/3.281</f>
-        <v>1.929289850655288</v>
+        <f>6/3.281</f>
+        <v>1.8287107589149649</v>
       </c>
       <c r="G34" s="41">
         <f>C34*(PI())*(D34)*E34*F34</f>
-        <v>1.2383005438991532</v>
+        <v>1.2408666469319718</v>
       </c>
       <c r="H34" s="42"/>
       <c r="I34" s="42"/>
@@ -5737,10 +5742,10 @@
       <c r="R34" s="25"/>
       <c r="S34" s="25"/>
     </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" s="60">
         <v>-3</v>
@@ -5776,7 +5781,7 @@
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="39" t="str">
         <f>B34</f>
@@ -5793,12 +5798,12 @@
         <v>0.23</v>
       </c>
       <c r="F36" s="61">
-        <f>4.33/3.281</f>
-        <v>1.3197195976836329</v>
+        <f>4/3.281</f>
+        <v>1.2191405059433098</v>
       </c>
       <c r="G36" s="41">
         <f>C36*(PI())*(D36)*E36*F36</f>
-        <v>0.64346492110193376</v>
+        <v>0.5944248693782298</v>
       </c>
       <c r="H36" s="42"/>
       <c r="I36" s="42"/>
@@ -5812,10 +5817,10 @@
       <c r="R36" s="25"/>
       <c r="S36" s="25"/>
     </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="60">
         <v>-2</v>
@@ -5851,10 +5856,10 @@
       <c r="R37" s="25"/>
       <c r="S37" s="25"/>
     </row>
-    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="42"/>
       <c r="B38" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" s="44"/>
       <c r="D38" s="45"/>
@@ -5862,17 +5867,17 @@
       <c r="F38" s="45"/>
       <c r="G38" s="33">
         <f>SUM(G34:G37)</f>
-        <v>1.5566106253545435</v>
+        <v>1.5101366766636579</v>
       </c>
       <c r="H38" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I38" s="33">
         <v>14362.76</v>
       </c>
       <c r="J38" s="46">
         <f>G38*I38</f>
-        <v>22357.224825417223</v>
+        <v>21689.73065411772</v>
       </c>
       <c r="K38" s="38"/>
       <c r="N38">
@@ -5888,10 +5893,10 @@
         <v>0.58473026516306004</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="42"/>
       <c r="B39" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C39" s="44"/>
       <c r="D39" s="45"/>
@@ -5902,11 +5907,11 @@
       <c r="I39" s="45"/>
       <c r="J39" s="47">
         <f>0.13*G38*10311.74</f>
-        <v>2086.6773264861499</v>
+        <v>2024.3777806485621</v>
       </c>
       <c r="K39" s="38"/>
     </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="42"/>
       <c r="B40" s="39"/>
       <c r="C40" s="44"/>
@@ -5919,12 +5924,12 @@
       <c r="J40" s="47"/>
       <c r="K40" s="38"/>
     </row>
-    <row r="41" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="18">
         <v>6</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="38"/>
       <c r="D41" s="40"/>
@@ -5943,10 +5948,10 @@
       <c r="R41" s="25"/>
       <c r="S41" s="25"/>
     </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C42" s="38">
         <f>(45+17.5)/2.5+1</f>
@@ -5982,10 +5987,10 @@
       <c r="R42" s="25"/>
       <c r="S42" s="25"/>
     </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18"/>
       <c r="B43" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43" s="38"/>
       <c r="D43" s="40"/>
@@ -5996,7 +6001,7 @@
         <v>65</v>
       </c>
       <c r="H43" s="42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I43" s="42">
         <v>6932.79</v>
@@ -6017,10 +6022,10 @@
       <c r="R43" s="25"/>
       <c r="S43" s="25"/>
     </row>
-    <row r="44" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C44" s="38"/>
       <c r="D44" s="40"/>
@@ -6042,7 +6047,7 @@
       <c r="R44" s="25"/>
       <c r="S44" s="25"/>
     </row>
-    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="39"/>
       <c r="C45" s="38"/>
@@ -6062,12 +6067,12 @@
       <c r="R45" s="25"/>
       <c r="S45" s="25"/>
     </row>
-    <row r="46" spans="1:19" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="18">
         <v>7</v>
       </c>
       <c r="B46" s="68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" s="29">
         <v>1</v>
@@ -6080,7 +6085,7 @@
         <v>1</v>
       </c>
       <c r="H46" s="69" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I46" s="23">
         <v>5000</v>
@@ -6094,7 +6099,7 @@
       <c r="R46" s="35"/>
       <c r="S46" s="35"/>
     </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
       <c r="B47" s="39"/>
       <c r="C47" s="38"/>
@@ -6114,7 +6119,7 @@
       <c r="R47" s="25"/>
       <c r="S47" s="25"/>
     </row>
-    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18">
         <v>8</v>
       </c>
@@ -6150,7 +6155,7 @@
       <c r="R48" s="25"/>
       <c r="S48" s="25"/>
     </row>
-    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18"/>
       <c r="B49" s="24"/>
       <c r="C49" s="19"/>
@@ -6170,7 +6175,7 @@
       <c r="R49" s="25"/>
       <c r="S49" s="25"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="42"/>
       <c r="B50" s="48" t="s">
         <v>17</v>
@@ -6184,11 +6189,11 @@
       <c r="I50" s="43"/>
       <c r="J50" s="43">
         <f>SUM(J10:J48)</f>
-        <v>560165.0746088404</v>
+        <v>559435.28089170333</v>
       </c>
       <c r="K50" s="38"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="62"/>
       <c r="B51" s="65"/>
       <c r="C51" s="66"/>
@@ -6201,16 +6206,16 @@
       <c r="J51" s="64"/>
       <c r="K51" s="59"/>
     </row>
-    <row r="52" spans="1:19" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="52"/>
       <c r="B52" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" s="71">
+        <v>60</v>
+      </c>
+      <c r="C52" s="77">
         <f>J50</f>
-        <v>560165.0746088404</v>
-      </c>
-      <c r="D52" s="71"/>
+        <v>559435.28089170333</v>
+      </c>
+      <c r="D52" s="77"/>
       <c r="E52" s="41">
         <v>100</v>
       </c>
@@ -6221,15 +6226,15 @@
       <c r="J52" s="56"/>
       <c r="K52" s="57"/>
     </row>
-    <row r="53" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="58"/>
       <c r="B53" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C53" s="74">
+      <c r="C53" s="80">
         <v>500000</v>
       </c>
-      <c r="D53" s="74"/>
+      <c r="D53" s="80"/>
       <c r="E53" s="41"/>
       <c r="F53" s="51"/>
       <c r="G53" s="50"/>
@@ -6238,16 +6243,16 @@
       <c r="J53" s="50"/>
       <c r="K53" s="51"/>
     </row>
-    <row r="54" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="58"/>
       <c r="B54" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C54" s="74">
+      <c r="C54" s="80">
         <f>0.85*C52</f>
-        <v>476140.31341751432</v>
-      </c>
-      <c r="D54" s="74"/>
+        <v>475519.98875794781</v>
+      </c>
+      <c r="D54" s="80"/>
       <c r="E54" s="41">
         <f>C54/C52*100</f>
         <v>85</v>
@@ -6259,16 +6264,16 @@
       <c r="J54" s="50"/>
       <c r="K54" s="51"/>
     </row>
-    <row r="55" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="58"/>
       <c r="B55" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C55" s="71">
+      <c r="C55" s="77">
         <f>C52-C54</f>
-        <v>84024.761191326077</v>
-      </c>
-      <c r="D55" s="71"/>
+        <v>83915.292133755516</v>
+      </c>
+      <c r="D55" s="77"/>
       <c r="E55" s="41">
         <f>100-E54</f>
         <v>15</v>
@@ -6280,16 +6285,16 @@
       <c r="J55" s="50"/>
       <c r="K55" s="51"/>
     </row>
-    <row r="56" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="58"/>
       <c r="B56" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="71">
+      <c r="C56" s="77">
         <f>C53*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D56" s="71"/>
+      <c r="D56" s="77"/>
       <c r="E56" s="41">
         <v>3</v>
       </c>
@@ -6300,16 +6305,16 @@
       <c r="J56" s="50"/>
       <c r="K56" s="51"/>
     </row>
-    <row r="57" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="58"/>
       <c r="B57" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C57" s="71">
+      <c r="C57" s="77">
         <f>C53*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D57" s="71"/>
+      <c r="D57" s="77"/>
       <c r="E57" s="41">
         <v>2</v>
       </c>
@@ -6320,7 +6325,7 @@
       <c r="J57" s="50"/>
       <c r="K57" s="51"/>
     </row>
-    <row r="58" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="59"/>
       <c r="B58" s="59"/>
       <c r="C58" s="59"/>
@@ -6333,68 +6338,69 @@
       <c r="J58" s="59"/>
       <c r="K58" s="59"/>
     </row>
-    <row r="59" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="102" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="103" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="104" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="105" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="106" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="107" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="108" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="109" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="110" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="111" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="112" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="113" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="114" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:19" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="C57:D57"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="G7:K7"/>
     <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="C54:D54"/>
@@ -6405,7 +6411,6 @@
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
@@ -6415,8 +6420,5 @@
 Er. Milan Phuyal&amp;RApproved By:
 Er. Prakash Singh Saud</oddFooter>
   </headerFooter>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="35" max="10" man="1"/>
-  </rowBreaks>
 </worksheet>
 </file>
</xml_diff>